<commit_message>
[PHOENIX-5854] UI trade license changes
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/tradeLicenseTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="729" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,6 @@
     <t>Permanent</t>
   </si>
   <si>
-    <t>01/03/2017</t>
-  </si>
-  <si>
     <t>locality</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>1016092139</t>
+  </si>
+  <si>
+    <t>01/04/2017</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -659,10 +659,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>14</v>
@@ -673,13 +673,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>16</v>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -765,7 +765,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[PHOENIX-5854] added few more scenarios for renewal of license
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/tradeLicenseTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="729" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>dataName</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>TL/08360/2016</t>
-  </si>
-  <si>
-    <t>Veterinary Trades</t>
   </si>
   <si>
     <t xml:space="preserve">01987-2017-HB </t>
@@ -659,10 +656,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>14</v>
@@ -673,13 +670,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>16</v>
@@ -699,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -750,13 +747,13 @@
         <v>25</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="7">
         <v>100</v>
@@ -765,7 +762,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -773,7 +770,7 @@
         <v>26</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -861,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -891,7 +888,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +924,7 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>